<commit_message>
update data March 24
</commit_message>
<xml_diff>
--- a/inst/extdata/China fossil fuel imports from Russia.xlsx
+++ b/inst/extdata/China fossil fuel imports from Russia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\CREA-China\monthly snapshot\wind data templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DFAD348-4196-4971-BAF6-2A5077A12D3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7E1E41-4F4C-43C4-8A68-9DC96D61791A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="10425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Volume of Imports_ Steam Coal_ " sheetId="1" r:id="rId1"/>
@@ -496,9 +496,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N319"/>
+  <dimension ref="A1:N320"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A304" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A304" workbookViewId="0">
+      <selection activeCell="F315" sqref="F315"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -14112,7 +14114,7 @@
         <v>648165872</v>
       </c>
       <c r="M310" s="3">
-        <v>7682835020</v>
+        <v>7682555619</v>
       </c>
       <c r="N310" s="3">
         <v>4237784928</v>
@@ -14126,7 +14128,7 @@
         <v>4374953.165</v>
       </c>
       <c r="C311" s="3">
-        <v>714223110</v>
+        <v>714230766</v>
       </c>
       <c r="D311" s="3">
         <v>2282846.5299999998</v>
@@ -14135,7 +14137,7 @@
         <v>457555753</v>
       </c>
       <c r="F311" s="3">
-        <v>1596351645</v>
+        <v>1596359301</v>
       </c>
       <c r="G311" s="3">
         <v>8830060.2550000008</v>
@@ -14159,7 +14161,7 @@
         <v>9606059137</v>
       </c>
       <c r="N311" s="3">
-        <v>5185182200</v>
+        <v>5185216488</v>
       </c>
     </row>
     <row r="312" spans="1:14">
@@ -14179,7 +14181,7 @@
         <v>548744915</v>
       </c>
       <c r="F312" s="3">
-        <v>1352077364</v>
+        <v>1352156465</v>
       </c>
       <c r="G312" s="3">
         <v>8094939.2800000003</v>
@@ -14211,22 +14213,22 @@
         <v>45077</v>
       </c>
       <c r="B313" s="3">
-        <v>5046637.909</v>
+        <v>5046632.909</v>
       </c>
       <c r="C313" s="3">
         <v>651888954</v>
       </c>
       <c r="D313" s="3">
-        <v>1938657.655</v>
+        <v>1938654.655</v>
       </c>
       <c r="E313" s="3">
         <v>327531282</v>
       </c>
       <c r="F313" s="3">
-        <v>1264499918</v>
+        <v>1261028485</v>
       </c>
       <c r="G313" s="3">
-        <v>8834120.6510000005</v>
+        <v>8834112.6510000005</v>
       </c>
       <c r="H313" s="3">
         <v>1635691161</v>
@@ -14235,7 +14237,7 @@
         <v>889073429</v>
       </c>
       <c r="J313" s="3">
-        <v>3765393226</v>
+        <v>3766131348</v>
       </c>
       <c r="K313" s="3">
         <v>0</v>
@@ -14244,7 +14246,7 @@
         <v>480749492</v>
       </c>
       <c r="M313" s="3">
-        <v>9704484829</v>
+        <v>9704129565</v>
       </c>
       <c r="N313" s="3">
         <v>5238533428</v>
@@ -14258,16 +14260,16 @@
         <v>5859869.3159999996</v>
       </c>
       <c r="C314" s="3">
-        <v>674576622</v>
+        <v>674810327</v>
       </c>
       <c r="D314" s="3">
         <v>2190490.0619999999</v>
       </c>
       <c r="E314" s="3">
-        <v>309166889</v>
+        <v>311925456</v>
       </c>
       <c r="F314" s="3">
-        <v>1313629169</v>
+        <v>1310571591</v>
       </c>
       <c r="G314" s="3">
         <v>10578601.704</v>
@@ -14279,7 +14281,7 @@
         <v>849815572</v>
       </c>
       <c r="J314" s="3">
-        <v>3318624835</v>
+        <v>3320507486</v>
       </c>
       <c r="K314" s="3">
         <v>0</v>
@@ -14288,10 +14290,10 @@
         <v>573460106</v>
       </c>
       <c r="M314" s="3">
-        <v>10494579569</v>
+        <v>10493989499</v>
       </c>
       <c r="N314" s="3">
-        <v>5443068707</v>
+        <v>5443481794</v>
       </c>
     </row>
     <row r="315" spans="1:14">
@@ -14299,19 +14301,19 @@
         <v>45138</v>
       </c>
       <c r="B315" s="3">
-        <v>5653999.9170000004</v>
+        <v>5724999.9170000004</v>
       </c>
       <c r="C315" s="3">
-        <v>567000588</v>
+        <v>573025675</v>
       </c>
       <c r="D315" s="3">
         <v>1606198.2379999999</v>
       </c>
       <c r="E315" s="3">
-        <v>205996832</v>
+        <v>212038070</v>
       </c>
       <c r="F315" s="3">
-        <v>963660677</v>
+        <v>968573703</v>
       </c>
       <c r="G315" s="3">
         <v>8992095.9100000001</v>
@@ -14323,7 +14325,7 @@
         <v>579942483</v>
       </c>
       <c r="J315" s="3">
-        <v>3159790687</v>
+        <v>3159828252</v>
       </c>
       <c r="K315" s="3">
         <v>0</v>
@@ -14332,10 +14334,10 @@
         <v>555570230</v>
       </c>
       <c r="M315" s="3">
-        <v>8060784639</v>
+        <v>8060767087</v>
       </c>
       <c r="N315" s="3">
-        <v>4256627909</v>
+        <v>4261482288</v>
       </c>
     </row>
     <row r="316" spans="1:14">
@@ -14343,31 +14345,31 @@
         <v>45169</v>
       </c>
       <c r="B316" s="3">
-        <v>5875463.5669999998</v>
+        <v>5875458.4680000003</v>
       </c>
       <c r="C316" s="3">
-        <v>551572942</v>
+        <v>551225013</v>
       </c>
       <c r="D316" s="3">
-        <v>2260977.66</v>
+        <v>2260972.16</v>
       </c>
       <c r="E316" s="3">
-        <v>309029609</v>
+        <v>310355173</v>
       </c>
       <c r="F316" s="3">
-        <v>1073573178</v>
+        <v>1075430990</v>
       </c>
       <c r="G316" s="3">
-        <v>9964077.9570000004</v>
+        <v>9964067.3579999991</v>
       </c>
       <c r="H316" s="3">
         <v>1672375204</v>
       </c>
       <c r="I316" s="3">
-        <v>994273631</v>
+        <v>992845331</v>
       </c>
       <c r="J316" s="3">
-        <v>3504986409</v>
+        <v>3505698584</v>
       </c>
       <c r="K316" s="3">
         <v>0</v>
@@ -14376,10 +14378,10 @@
         <v>519326596</v>
       </c>
       <c r="M316" s="3">
-        <v>10541981341</v>
+        <v>10541721938</v>
       </c>
       <c r="N316" s="3">
-        <v>5976587626</v>
+        <v>6004367341</v>
       </c>
     </row>
     <row r="317" spans="1:14">
@@ -14390,16 +14392,16 @@
         <v>5157982.3219999997</v>
       </c>
       <c r="C317" s="3">
-        <v>494244237</v>
+        <v>494555109</v>
       </c>
       <c r="D317" s="3">
         <v>2593896.75</v>
       </c>
       <c r="E317" s="3">
-        <v>362294551</v>
+        <v>362312257</v>
       </c>
       <c r="F317" s="3">
-        <v>1013622977</v>
+        <v>1015558695</v>
       </c>
       <c r="G317" s="3">
         <v>9169111.2699999996</v>
@@ -14411,7 +14413,7 @@
         <v>739527432</v>
       </c>
       <c r="J317" s="3">
-        <v>3155278329</v>
+        <v>3153792997</v>
       </c>
       <c r="K317" s="3">
         <v>0</v>
@@ -14420,10 +14422,10 @@
         <v>519747239</v>
       </c>
       <c r="M317" s="3">
-        <v>8735926543</v>
+        <v>8736032161</v>
       </c>
       <c r="N317" s="3">
-        <v>5396952222</v>
+        <v>5426633373</v>
       </c>
     </row>
     <row r="318" spans="1:14">
@@ -14431,22 +14433,22 @@
         <v>45230</v>
       </c>
       <c r="B318" s="3">
-        <v>4149465.7949999999</v>
+        <v>4149185.7949999999</v>
       </c>
       <c r="C318" s="3">
-        <v>409706378</v>
+        <v>409639067</v>
       </c>
       <c r="D318" s="3">
         <v>1831562.2</v>
       </c>
       <c r="E318" s="3">
-        <v>302270294</v>
+        <v>302658775</v>
       </c>
       <c r="F318" s="3">
-        <v>922192760</v>
+        <v>923702341</v>
       </c>
       <c r="G318" s="3">
-        <v>7628481.9850000003</v>
+        <v>7628201.9850000003</v>
       </c>
       <c r="H318" s="3">
         <v>1339100836</v>
@@ -14455,7 +14457,7 @@
         <v>739594629</v>
       </c>
       <c r="J318" s="3">
-        <v>2914508827</v>
+        <v>2911655881</v>
       </c>
       <c r="K318" s="3">
         <v>0</v>
@@ -14464,10 +14466,10 @@
         <v>386008355</v>
       </c>
       <c r="M318" s="3">
-        <v>8535444969</v>
+        <v>8534782775</v>
       </c>
       <c r="N318" s="3">
-        <v>5502769679</v>
+        <v>5533272637</v>
       </c>
     </row>
     <row r="319" spans="1:14">
@@ -14475,31 +14477,31 @@
         <v>45260</v>
       </c>
       <c r="B319" s="3">
-        <v>3636590.29</v>
+        <v>3636675.89</v>
       </c>
       <c r="C319" s="3">
-        <v>412033504</v>
+        <v>411866953</v>
       </c>
       <c r="D319" s="3">
-        <v>1923657.9650000001</v>
+        <v>1923696.9650000001</v>
       </c>
       <c r="E319" s="3">
-        <v>311795252</v>
+        <v>313966609</v>
       </c>
       <c r="F319" s="3">
-        <v>953995002</v>
+        <v>958762597</v>
       </c>
       <c r="G319" s="3">
-        <v>7306207.9579999996</v>
+        <v>7306332.5580000002</v>
       </c>
       <c r="H319" s="3">
         <v>1565388170</v>
       </c>
       <c r="I319" s="3">
-        <v>621473716</v>
+        <v>609571153</v>
       </c>
       <c r="J319" s="3">
-        <v>4217387112</v>
+        <v>4187667201</v>
       </c>
       <c r="K319" s="3">
         <v>0</v>
@@ -14508,10 +14510,54 @@
         <v>518947875</v>
       </c>
       <c r="M319" s="3">
-        <v>9000809208</v>
+        <v>8999568903</v>
       </c>
       <c r="N319" s="3">
-        <v>5537189413</v>
+        <v>5545020618</v>
+      </c>
+    </row>
+    <row r="320" spans="1:14">
+      <c r="A320" s="2">
+        <v>45291</v>
+      </c>
+      <c r="B320" s="3">
+        <v>3389292.7050000001</v>
+      </c>
+      <c r="C320" s="3">
+        <v>373722796</v>
+      </c>
+      <c r="D320" s="3">
+        <v>2425503.2000000002</v>
+      </c>
+      <c r="E320" s="3">
+        <v>423520291</v>
+      </c>
+      <c r="F320" s="3">
+        <v>1042735863</v>
+      </c>
+      <c r="G320" s="3">
+        <v>7592889.1310000001</v>
+      </c>
+      <c r="H320" s="3">
+        <v>1607432321</v>
+      </c>
+      <c r="I320" s="3">
+        <v>519221118</v>
+      </c>
+      <c r="J320" s="3">
+        <v>5851319211</v>
+      </c>
+      <c r="K320" s="3">
+        <v>0</v>
+      </c>
+      <c r="L320" s="3">
+        <v>549402142</v>
+      </c>
+      <c r="M320" s="3">
+        <v>9561014006</v>
+      </c>
+      <c r="N320" s="3">
+        <v>5525313310</v>
       </c>
     </row>
   </sheetData>

</xml_diff>